<commit_message>
Cập nhật file Requirements.xlsx
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TIẾN ĐỘ HỌC TẬP HK242\THIẾT KẾ HỆ THỐNG NHÚNG(CẢI THIỆN)\BLT_THIẾT KẾ HỆ THỐNG NHÚNG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{16DFBE68-B714-404F-B4F8-DF02A9572FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B984A4F2-C56D-4644-9432-DDD0C53DCA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{40329A33-A4F3-4627-8CB6-47159A48CFF6}"/>
   </bookViews>
@@ -25,90 +25,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>1. Fire Detection and Alerting</t>
   </si>
   <si>
-    <t>1.1 The system shall detect fire incidents and alert relevant authorities.</t>
-  </si>
-  <si>
-    <t>1.2 The system shall send notifications to designated personnel.</t>
-  </si>
-  <si>
-    <t>1.2.2 The system shall include real-time GPS location in the alerts with an NEO-6M GPS module.</t>
-  </si>
-  <si>
-    <t>2. Communication and GPS Tracking</t>
-  </si>
-  <si>
     <t>2.1 The system shall use an STM32F103C8T6 microcontroller for processing.</t>
   </si>
   <si>
-    <t>2.3 The system shall acquire and send GPS coordinates with an accuracy of ±2.5 meters when a fire is detected.</t>
-  </si>
-  <si>
     <t>3. Emergency Response Features</t>
   </si>
   <si>
     <t>3.1 The system shall provide an emergency shutdown option for electrical systems within 5 seconds of detection.</t>
   </si>
   <si>
-    <t>3.2 The system shall activate emergency lighting (LED 10W) in case of power failure.</t>
-  </si>
-  <si>
-    <t>4. Connectivity and Reliability</t>
-  </si>
-  <si>
-    <t>4.1 The system shall operate independently of Wi-Fi networks.</t>
-  </si>
-  <si>
-    <t>4.2 The system shall maintain functionality even in case of network disruptions with a redundant GSM module.</t>
-  </si>
-  <si>
-    <t>5. User Interface and Monitoring</t>
-  </si>
-  <si>
-    <t>5.2 The system shall provide a web-based or mobile application for remote monitoring.</t>
-  </si>
-  <si>
-    <t>5.3 The system shall log up to 1000 fire incidents for later review.</t>
-  </si>
-  <si>
-    <t>6. Security and Safety</t>
-  </si>
-  <si>
-    <t>6.1 The system shall implement authentication to access remote monitoring features with a 6-digit PIN or biometric verification.</t>
-  </si>
-  <si>
-    <t>6.2 The system shall encrypt data transmission using AES-128 to ensure security.</t>
-  </si>
-  <si>
-    <t>6.3 The system shall comply with fire safety regulations such as NFPA 72 and IEC 61508.</t>
-  </si>
-  <si>
-    <t>5.1 The system shall have a LCD 1602 driver HD44780 for local monitoring.</t>
-  </si>
-  <si>
-    <t>1.2.1 The system shall send SMS alerts via a SIM800A module.</t>
-  </si>
-  <si>
-    <t>1.1.2 The system shall activate a local alarm with a buzzer (120 dB) and send remote notifications.</t>
-  </si>
-  <si>
-    <t>3.3 The system shall include a warning light (5W flashing light) to indicate emergency conditions.</t>
-  </si>
-  <si>
-    <t>4.3 The system shall have a 12V, 7Ah backup battery to ensure continuous operation for up to 8 hours. continuous operation for up to 8 hours.</t>
-  </si>
-  <si>
-    <t>Smoke and Gas Leak Monitoring, Fire and Explosion Alarm System</t>
-  </si>
-  <si>
     <t>2.2 The system shall use a SIM7680C 4G module to transmit alerts.</t>
   </si>
   <si>
-    <t>1.1.1 The system shall use smoke sensors (MQ-2), LM393 and heat sensors (DHT11) to detect fire.</t>
+    <t>FIRE ALARM SYSTEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   5. Power and Reliability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.1 The system shall detect fire incidents and alert relevant authorities.</t>
+  </si>
+  <si>
+    <t>3.2 The system shall include a warning light (5W flashing light) to indicate emergency conditions.</t>
+  </si>
+  <si>
+    <t>3.3 The system shall activate a water pump to suppress the fire when detection occurs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        1.1.1 The system shall use smoke sensors (MQ-2), LM393 and heat sensors (DHT11) to detect fire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        1.1.2 The system shall activate a local alarm with a buzzer (120 dB) and send remote notifications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        1.2.1 The system shall send SMS alerts via a SIM7680C module.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.2 The system shall send notifications to designated person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         3.1.1 The system shall activate emergency lighting (LED 10W) in case of power failure.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         3.3.1 The water pump shall have a minimum power rating of 50W to ensure adequate water flow.</t>
+  </si>
+  <si>
+    <t>4. User Interface and Monitoring</t>
+  </si>
+  <si>
+    <t>4.1 The system shall have a LCD 1602 driver HD44780 for local monitoring.</t>
+  </si>
+  <si>
+    <t>The Fire Alarm System is designed to detect fire incidents and provide 
+immediate alerts while activating emergency response mechanisms. The system relies on an STM32 microcontroller and a SIM module to send notifications via SMS to designated phone numbers.
+Input: Gas sensor, Temp&amp;humid sensor, Flame sensor, Button...
+Output: LCD display, Buzzer, Light, Water Pump, Relay, Sim 4G...</t>
+  </si>
+  <si>
+    <t>2. Communication</t>
+  </si>
+  <si>
+    <t>5.1 The system shall be powered by the main power grid</t>
+  </si>
+  <si>
+    <t>5.3 The system shall continue operation in case of power failure for at least 24 hours using a backup battery.</t>
+  </si>
+  <si>
+    <t>5.2 The system shall be powered by a stable power source with battery backup.</t>
   </si>
 </sst>
 </file>
@@ -152,13 +140,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,21 +466,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C61E53-F6BD-4739-B455-DEC175776146}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="60.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -498,72 +496,69 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
+      <c r="A14" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
+      <c r="A16" s="1"/>
+      <c r="B16" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -573,90 +568,53 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>11</v>
+      <c r="A21" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
+      <c r="A24" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>13</v>
+      <c r="A25" s="1"/>
+      <c r="B25" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>20</v>
+      <c r="B26" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1" t="s">
-        <v>19</v>
+      <c r="B27" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>